<commit_message>
DO NOT PULL unless you want to work on the submit button
bug!
</commit_message>
<xml_diff>
--- a/Requirements Implementation Status.xlsx
+++ b/Requirements Implementation Status.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F5F1C8-0164-480F-8A78-6743997072DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>1.   All pages will be of type.php</t>
   </si>
@@ -189,7 +188,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -199,7 +198,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -215,7 +214,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -225,7 +224,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -271,23 +270,29 @@
   <si>
     <t>right now we are displaying the last product in the list</t>
   </si>
+  <si>
+    <t>Guy</t>
+  </si>
+  <si>
+    <t>Alon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -295,7 +300,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -304,7 +309,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -313,14 +318,14 @@
       <u/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -371,9 +376,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -410,11 +412,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="טוב" xfId="1" builtinId="26"/>
+    <cellStyle name="רע" xfId="2" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -684,27 +689,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="84.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -712,333 +717,352 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="B9" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="32" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="14" t="s">
+    <row r="40" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A40" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="14" t="s">
+      <c r="B40" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+      <c r="B41" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="1:2" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
+    <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A54" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="14" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="14" t="s">
+    <row r="57" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="29.25" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" ht="57" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:B13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Notification when upload new flights
works only if you have the new db
</commit_message>
<xml_diff>
--- a/Requirements Implementation Status.xlsx
+++ b/Requirements Implementation Status.xlsx
@@ -362,7 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -390,9 +390,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -699,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -733,7 +730,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -753,36 +750,36 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="15"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="16"/>
-    </row>
-    <row r="13" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
@@ -790,7 +787,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -803,17 +800,17 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -868,7 +865,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -876,7 +873,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -884,7 +881,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>59</v>
       </c>
     </row>
@@ -894,32 +891,32 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>62</v>
       </c>
     </row>
@@ -940,78 +937,78 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="17"/>
+      <c r="B53" s="16"/>
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1029,12 +1026,12 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="13" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>